<commit_message>
added myers trauma 10/15 and holiday
</commit_message>
<xml_diff>
--- a/resident_holiday_requests.xlsx
+++ b/resident_holiday_requests.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="27">
   <si>
     <t>Dyer</t>
   </si>
@@ -147,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -156,9 +156,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,7 +474,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -508,16 +505,16 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -525,16 +522,16 @@
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -610,10 +607,10 @@
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -729,10 +726,18 @@
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
@@ -745,10 +750,10 @@
         <v>21</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.4">

</xml_diff>